<commit_message>
Revert "Merge branch 'master' of https://github.com/BI-DSS/ERPMVC"
This reverts commit c4f6bb85ae2d91d576d601e0a6492490d94e67c0, reversing
changes made to 4a69231dc6976264d03b417269f67ddf85de3196.
</commit_message>
<xml_diff>
--- a/ERPMVC/Spreadsheet.xlsx
+++ b/ERPMVC/Spreadsheet.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView/>
+    <workbookView activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Evaluation Warning" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr fullPrecision="1" calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32" count="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33" count="34">
   <si>
     <t>InvoiceCalculationId</t>
   </si>
@@ -106,20 +107,20 @@
     <t>Cafe Pergamino</t>
   </si>
   <si>
-    <t>18cf60aa-698a-45ca-afd6-8e9e66b162cb</t>
+    <t>ee36f34b-88cf-453a-aa70-6d2b8963fd46</t>
   </si>
   <si>
     <t>erp@bi-dss.com</t>
+  </si>
+  <si>
+    <t>Created with a trial version of Syncfusion Essential XlsIO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -142,6 +143,17 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <name val="Calibri"/>
       <charset val="0"/>
     </font>
@@ -169,7 +181,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyFill="0" applyProtection="0"/>
@@ -193,7 +205,8 @@
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,7 +226,7 @@
   <sheetPr/>
   <dimension ref="A2:AB3"/>
   <sheetViews>
-    <sheetView view="normal" tabSelected="1" workbookViewId="0">
+    <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -307,10 +320,10 @@
     </row>
     <row r="3" spans="1:28">
       <c r="A3">
-        <v>10126</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>43751.664581122684</v>
+        <v>43742.055485115743</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -328,7 +341,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="I3">
         <v>22</v>
@@ -340,16 +353,16 @@
         <v>30</v>
       </c>
       <c r="L3">
-        <v>43.4</v>
+        <v>23</v>
       </c>
       <c r="M3">
         <v>32.98</v>
       </c>
       <c r="N3">
-        <v>1431.3319999999999</v>
+        <v>758.54</v>
       </c>
       <c r="O3">
-        <v>28.62664</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <v>1099.3333333333333</v>
@@ -364,10 +377,10 @@
         <v>0.03</v>
       </c>
       <c r="T3">
-        <v>44.268</v>
+        <v>23.46</v>
       </c>
       <c r="U3">
-        <v>0.88536</v>
+        <v>0</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -382,14 +395,39 @@
         <v>31</v>
       </c>
       <c r="AA3" s="1">
-        <v>43769.8642193287</v>
+        <v>43766.484943888892</v>
       </c>
       <c r="AB3" s="1">
-        <v>43769.8642193287</v>
+        <v>43766.484943888892</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <tabColor rgb="FFFF4500"/>
+  </sheetPr>
+  <dimension ref="A10"/>
+  <sheetViews>
+    <sheetView view="normal" tabSelected="1" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="10" spans="1:1" ht="25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="F7F5" sheet="1" objects="1" scenarios="1" pivotTables="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>
+</worksheet>
 </file>
</xml_diff>